<commit_message>
before messing up css
</commit_message>
<xml_diff>
--- a/misc/repsonsiveness.xlsx
+++ b/misc/repsonsiveness.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sync\Code\Python\autosyntax_afterebcrash\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B4532B19-3C2F-4E66-944C-913A579F4895}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB367309-8857-4801-87A3-8C4B048FF1E8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8235" xr2:uid="{2A8C8114-1B4B-42B4-8FD9-393781E7875E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t>body</t>
   </si>
@@ -33,12 +33,6 @@
     <t>space</t>
   </si>
   <si>
-    <t>continue-arrow</t>
-  </si>
-  <si>
-    <t>continue_arrow:hover</t>
-  </si>
-  <si>
     <t>work</t>
   </si>
   <si>
@@ -54,14 +48,6 @@
     <t>600 height 658</t>
   </si>
   <si>
-    <t>bottom, height, left, width
-10% 60px 50% 60px</t>
-  </si>
-  <si>
-    <t>height, left, width
-63px 49.8% 63px</t>
-  </si>
-  <si>
     <t>6% 55px 50% 55px</t>
   </si>
   <si>
@@ -222,6 +208,35 @@
   </si>
   <si>
     <t>50px 30px 60px</t>
+  </si>
+  <si>
+    <t>continue_arrow:hover
+height, left, width</t>
+  </si>
+  <si>
+    <t>63px 49.8% 63px</t>
+  </si>
+  <si>
+    <t>10% 60px 50% 60px</t>
+  </si>
+  <si>
+    <t>continue-arrow
+bottom, height, left, width</t>
+  </si>
+  <si>
+    <t>width max</t>
+  </si>
+  <si>
+    <t>width_div_target</t>
+  </si>
+  <si>
+    <t>div_by_avg</t>
+  </si>
+  <si>
+    <t>fixer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVG C20:M20= </t>
   </si>
 </sst>
 </file>
@@ -273,13 +288,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,198 +613,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF41B39-4A61-431F-9E42-71199D694581}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E15" sqref="E15"/>
+      <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K9" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="N9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="P9" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
       <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" t="s">
         <v>42</v>
       </c>
-      <c r="J10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
+        <v>53</v>
+      </c>
+      <c r="O10" t="s">
         <v>43</v>
       </c>
-      <c r="M10" t="s">
-        <v>46</v>
-      </c>
-      <c r="N10" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" t="s">
-        <v>47</v>
-      </c>
       <c r="P10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -793,75 +818,75 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
         <v>29</v>
       </c>
-      <c r="G11" t="s">
-        <v>33</v>
-      </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" t="s">
+        <v>57</v>
+      </c>
+      <c r="P11" t="s">
         <v>43</v>
-      </c>
-      <c r="J11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" t="s">
-        <v>55</v>
-      </c>
-      <c r="N11" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="N12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="P12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -869,39 +894,304 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="N13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" t="s">
         <v>46</v>
       </c>
-      <c r="M14" t="s">
+      <c r="O14" t="s">
         <v>46</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>220</v>
+      </c>
+      <c r="D16">
+        <v>130</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>85</v>
+      </c>
+      <c r="G16">
+        <v>70</v>
+      </c>
+      <c r="H16">
+        <v>70</v>
+      </c>
+      <c r="I16">
+        <v>65</v>
+      </c>
+      <c r="J16">
         <v>50</v>
       </c>
-      <c r="O14" t="s">
-        <v>50</v>
-      </c>
-      <c r="P14" t="s">
-        <v>34</v>
+      <c r="K16">
+        <v>45</v>
+      </c>
+      <c r="L16">
+        <v>35</v>
+      </c>
+      <c r="M16">
+        <v>30</v>
+      </c>
+      <c r="N16">
+        <v>22</v>
+      </c>
+      <c r="O16">
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17">
+        <v>1300</v>
+      </c>
+      <c r="D17">
+        <v>1170</v>
+      </c>
+      <c r="E17">
+        <v>990</v>
+      </c>
+      <c r="F17">
+        <v>950</v>
+      </c>
+      <c r="G17">
+        <v>850</v>
+      </c>
+      <c r="H17">
+        <v>689</v>
+      </c>
+      <c r="I17">
+        <v>672</v>
+      </c>
+      <c r="J17">
+        <v>626</v>
+      </c>
+      <c r="K17">
+        <v>553</v>
+      </c>
+      <c r="L17">
+        <v>537</v>
+      </c>
+      <c r="M17">
+        <v>424</v>
+      </c>
+      <c r="N17">
+        <v>390</v>
+      </c>
+      <c r="O17">
+        <v>343</v>
+      </c>
+      <c r="P17">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18">
+        <f>(C16/C19)</f>
+        <v>1.886074102870483</v>
+      </c>
+      <c r="D18">
+        <f>(D16/D19)</f>
+        <v>1.2383314816826403</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:M18" si="0">(E16/E19)</f>
+        <v>1.1257558924387638</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.99718271946023151</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0.91782215701183922</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>1.1322914854282489</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>1.0780117809290843</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0.89017438779103542</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>0.90691546126847977</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>0.7263955618808785</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>0.78856014163753041</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19">
+        <f>(C17/AVERAGE(C20:M20))</f>
+        <v>116.64440949863751</v>
+      </c>
+      <c r="D19">
+        <f>(D17/AVERAGE(C20:M20))</f>
+        <v>104.97996854877377</v>
+      </c>
+      <c r="E19">
+        <f>(E17/AVERAGE(C20:M20))</f>
+        <v>88.829204156654725</v>
+      </c>
+      <c r="F19">
+        <f>(F17/AVERAGE(C20:M20))</f>
+        <v>85.240145402850487</v>
+      </c>
+      <c r="G19">
+        <f>(G17/AVERAGE(C20:M20))</f>
+        <v>76.26749851833992</v>
+      </c>
+      <c r="H19">
+        <f>(H17/AVERAGE(C20:M20))</f>
+        <v>61.821537034277881</v>
+      </c>
+      <c r="I19">
+        <f>(I17/AVERAGE(C20:M20))</f>
+        <v>60.296187063911084</v>
+      </c>
+      <c r="J19">
+        <f>(J17/AVERAGE(C20:M20))</f>
+        <v>56.168769497036216</v>
+      </c>
+      <c r="K19">
+        <f>(K17/AVERAGE(C20:M20))</f>
+        <v>49.618737271343498</v>
+      </c>
+      <c r="L19">
+        <f>(L17/AVERAGE(C20:M20))</f>
+        <v>48.183113769821801</v>
+      </c>
+      <c r="M19">
+        <f>(M17/AVERAGE(C20:M20))</f>
+        <v>38.044022790324853</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20">
+        <f>1300/250</f>
+        <v>5.2</v>
+      </c>
+      <c r="C20">
+        <f>(C17/C16)</f>
+        <v>5.9090909090909092</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:P20" si="1">(D17/D16)</f>
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>9.9</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>11.176470588235293</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>12.142857142857142</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>9.8428571428571434</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>10.338461538461539</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>12.52</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>12.28888888888889</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>15.342857142857143</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>14.133333333333333</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>17.727272727272727</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="1"/>
+        <v>22.866666666666667</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="1"/>
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f>AVERAGE(C20:M20)</f>
+        <v>11.144983335143763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>